<commit_message>
issue return tab added
</commit_message>
<xml_diff>
--- a/test_project/Issue_return.xlsx
+++ b/test_project/Issue_return.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,52 +436,107 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Weight returned</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Return Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Approval Date</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>APPROVAL NO.</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>SKU</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>PL No.</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Mine</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Price Code</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Lot Details (If Any)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Original weight</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Weight issued</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>SELECTION YES/NO</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>SELECTION CRITERIA</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>ASKING RATE</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>BROKER NAME</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>PARTY NAME</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
         </is>
       </c>
     </row>

</xml_diff>